<commit_message>
fix some typos (#88)
* fix some typos

* numero Galion in bold !
</commit_message>
<xml_diff>
--- a/static/files/stationnements.xlsx
+++ b/static/files/stationnements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E09827-43E9-CF46-9DA1-12CB1B3DC9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C685F8-10A6-BB44-B75B-BD41CFC27D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Stationnements" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>LOYER MAXIMUM conventionné de l’annexe en euros par mois</t>
   </si>
   <si>
-    <t>Garage Aérien</t>
-  </si>
-  <si>
     <t>Garage enterré</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>5. Vérifier le contenu téléversé dans l'application et enregistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
+  </si>
+  <si>
+    <t>Garage aérien</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>6</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1008,7 +1008,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
@@ -1026,9 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1042,17 +1040,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
@@ -1065,7 +1063,7 @@
       <c r="A7" s="14"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="0g4/dz0GA0X4EP39LJ2GjXXSslR+++820bKTgrON/8Aazxgl3yl3rQTWVMwP3CHr+tmjK8jj43/jI07o9BmFoA==" saltValue="DgPvZbS3Dt5DDfIV0guKVg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="NrdJVeeSQ4O0b3ijl93KuzKRABapYkCeOxFACVX/ZOWKUrXgZZmkNS6p+mdk2b3RRN4HvZ7FRuc50UGU/L+YGg==" saltValue="aYsNbNwirVdfbZpnR9zITQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
update the list of 'stationnements'
</commit_message>
<xml_diff>
--- a/static/files/stationnements.xlsx
+++ b/static/files/stationnements.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C685F8-10A6-BB44-B75B-BD41CFC27D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622A43ED-CA42-3345-8AA9-7456EEBDD5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="34700" yWindow="2060" windowWidth="27740" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Stationnements" sheetId="1" r:id="rId1"/>
     <sheet name="Notice" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Garage enterré</t>
   </si>
   <si>
-    <t>Place stationnement</t>
-  </si>
-  <si>
     <t>Nombre de stationnements</t>
   </si>
   <si>
@@ -81,6 +78,21 @@
   </si>
   <si>
     <t>Garage aérien</t>
+  </si>
+  <si>
+    <t>Garage boxé simple</t>
+  </si>
+  <si>
+    <t>Garage boxé double</t>
+  </si>
+  <si>
+    <t>Place de stationnement</t>
+  </si>
+  <si>
+    <t>Parking extérieur privatif</t>
+  </si>
+  <si>
+    <t>Parking en sous-sol ou en superstructure</t>
   </si>
 </sst>
 </file>
@@ -242,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -261,7 +273,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -358,8 +369,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A4" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:A4" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A8" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A8" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Type de stationnement" dataDxfId="0"/>
   </tableColumns>
@@ -666,9 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -679,8 +688,8 @@
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>11</v>
+      <c r="B1" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>6</v>
@@ -690,29 +699,29 @@
       <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
-      <c r="B3" s="15"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="16"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
-      <c r="B5" s="15"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
-      <c r="B6" s="16"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="12"/>
       <c r="D6" s="5"/>
       <c r="I6" s="5"/>
@@ -721,7 +730,7 @@
     </row>
     <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
-      <c r="B7" s="15"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="11"/>
       <c r="D7" s="5"/>
       <c r="I7" s="5"/>
@@ -730,222 +739,222 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
-      <c r="B8" s="16"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" s="15"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
-      <c r="B10" s="16"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
-      <c r="B11" s="15"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
-      <c r="B12" s="16"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
-      <c r="B13" s="15"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
-      <c r="B14" s="16"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
-      <c r="B15" s="15"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="11"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
-      <c r="B16" s="16"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
-      <c r="B17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="11"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
-      <c r="B18" s="16"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
-      <c r="B19" s="15"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
-      <c r="B20" s="16"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
-      <c r="B21" s="15"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="11"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
-      <c r="B22" s="16"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
-      <c r="B23" s="15"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
-      <c r="B24" s="16"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
-      <c r="B25" s="15"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
-      <c r="B26" s="16"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
-      <c r="B27" s="15"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
-      <c r="B28" s="16"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
-      <c r="B29" s="15"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="11"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
-      <c r="B30" s="16"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="12"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
-      <c r="B31" s="15"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
-      <c r="B32" s="16"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
-      <c r="B33" s="15"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
-      <c r="B34" s="16"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
-      <c r="B35" s="15"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="11"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
-      <c r="B36" s="16"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
-      <c r="B37" s="15"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="11"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
-      <c r="B38" s="16"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
-      <c r="B39" s="15"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="11"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
-      <c r="B40" s="16"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="12"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
-      <c r="B41" s="15"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="11"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
-      <c r="B42" s="16"/>
+      <c r="B42" s="15"/>
       <c r="C42" s="12"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
-      <c r="B43" s="15"/>
+      <c r="B43" s="14"/>
       <c r="C43" s="11"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
-      <c r="B44" s="16"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="12"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="8"/>
-      <c r="B45" s="15"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="11"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
-      <c r="B46" s="16"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="12"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="8"/>
-      <c r="B47" s="15"/>
+      <c r="B47" s="14"/>
       <c r="C47" s="11"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
-      <c r="B48" s="16"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="12"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="8"/>
-      <c r="B49" s="15"/>
+      <c r="B49" s="14"/>
       <c r="C49" s="11"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
-      <c r="B50" s="16"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="12"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
-      <c r="B51" s="17"/>
+      <c r="B51" s="16"/>
       <c r="C51" s="13"/>
     </row>
   </sheetData>
@@ -959,7 +968,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0632B4FB-3670-0342-8506-5DC3D8077703}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$4</xm:f>
+            <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A51</xm:sqref>
         </x14:dataValidation>
@@ -993,7 +1002,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1008,7 +1017,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
@@ -1024,7 +1033,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1040,7 +1049,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -1050,20 +1059,31 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NrdJVeeSQ4O0b3ijl93KuzKRABapYkCeOxFACVX/ZOWKUrXgZZmkNS6p+mdk2b3RRN4HvZ7FRuc50UGU/L+YGg==" saltValue="aYsNbNwirVdfbZpnR9zITQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FpFaiAt/hj0mRaeMQbB7SwPHtnqdpuLITDAqPUXBp8SuV4Wlwra5XV/V/t2i0Sbqawe5xjZ5939KAYfLbYVJpg==" saltValue="UA3tAN5V2NAz5u+7HUg5VA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
update the list of 'stationnements' (#114)
</commit_message>
<xml_diff>
--- a/static/files/stationnements.xlsx
+++ b/static/files/stationnements.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C685F8-10A6-BB44-B75B-BD41CFC27D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622A43ED-CA42-3345-8AA9-7456EEBDD5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="34700" yWindow="2060" windowWidth="27740" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Stationnements" sheetId="1" r:id="rId1"/>
     <sheet name="Notice" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Garage enterré</t>
   </si>
   <si>
-    <t>Place stationnement</t>
-  </si>
-  <si>
     <t>Nombre de stationnements</t>
   </si>
   <si>
@@ -81,6 +78,21 @@
   </si>
   <si>
     <t>Garage aérien</t>
+  </si>
+  <si>
+    <t>Garage boxé simple</t>
+  </si>
+  <si>
+    <t>Garage boxé double</t>
+  </si>
+  <si>
+    <t>Place de stationnement</t>
+  </si>
+  <si>
+    <t>Parking extérieur privatif</t>
+  </si>
+  <si>
+    <t>Parking en sous-sol ou en superstructure</t>
   </si>
 </sst>
 </file>
@@ -242,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -261,7 +273,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -358,8 +369,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A4" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:A4" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A8" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A8" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Type de stationnement" dataDxfId="0"/>
   </tableColumns>
@@ -666,9 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -679,8 +688,8 @@
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>11</v>
+      <c r="B1" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>6</v>
@@ -690,29 +699,29 @@
       <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
-      <c r="B3" s="15"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="16"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
-      <c r="B5" s="15"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
-      <c r="B6" s="16"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="12"/>
       <c r="D6" s="5"/>
       <c r="I6" s="5"/>
@@ -721,7 +730,7 @@
     </row>
     <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
-      <c r="B7" s="15"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="11"/>
       <c r="D7" s="5"/>
       <c r="I7" s="5"/>
@@ -730,222 +739,222 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
-      <c r="B8" s="16"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" s="15"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
-      <c r="B10" s="16"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
-      <c r="B11" s="15"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
-      <c r="B12" s="16"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
-      <c r="B13" s="15"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
-      <c r="B14" s="16"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
-      <c r="B15" s="15"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="11"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
-      <c r="B16" s="16"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
-      <c r="B17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="11"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
-      <c r="B18" s="16"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
-      <c r="B19" s="15"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
-      <c r="B20" s="16"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
-      <c r="B21" s="15"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="11"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
-      <c r="B22" s="16"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
-      <c r="B23" s="15"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
-      <c r="B24" s="16"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
-      <c r="B25" s="15"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
-      <c r="B26" s="16"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
-      <c r="B27" s="15"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
-      <c r="B28" s="16"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
-      <c r="B29" s="15"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="11"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
-      <c r="B30" s="16"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="12"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
-      <c r="B31" s="15"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
-      <c r="B32" s="16"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
-      <c r="B33" s="15"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
-      <c r="B34" s="16"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
-      <c r="B35" s="15"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="11"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
-      <c r="B36" s="16"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
-      <c r="B37" s="15"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="11"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
-      <c r="B38" s="16"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
-      <c r="B39" s="15"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="11"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
-      <c r="B40" s="16"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="12"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
-      <c r="B41" s="15"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="11"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
-      <c r="B42" s="16"/>
+      <c r="B42" s="15"/>
       <c r="C42" s="12"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
-      <c r="B43" s="15"/>
+      <c r="B43" s="14"/>
       <c r="C43" s="11"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
-      <c r="B44" s="16"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="12"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="8"/>
-      <c r="B45" s="15"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="11"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
-      <c r="B46" s="16"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="12"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="8"/>
-      <c r="B47" s="15"/>
+      <c r="B47" s="14"/>
       <c r="C47" s="11"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
-      <c r="B48" s="16"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="12"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="8"/>
-      <c r="B49" s="15"/>
+      <c r="B49" s="14"/>
       <c r="C49" s="11"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
-      <c r="B50" s="16"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="12"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
-      <c r="B51" s="17"/>
+      <c r="B51" s="16"/>
       <c r="C51" s="13"/>
     </row>
   </sheetData>
@@ -959,7 +968,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0632B4FB-3670-0342-8506-5DC3D8077703}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$4</xm:f>
+            <xm:f>Data!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A51</xm:sqref>
         </x14:dataValidation>
@@ -993,7 +1002,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1008,7 +1017,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
@@ -1024,7 +1033,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1040,7 +1049,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -1050,20 +1059,31 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NrdJVeeSQ4O0b3ijl93KuzKRABapYkCeOxFACVX/ZOWKUrXgZZmkNS6p+mdk2b3RRN4HvZ7FRuc50UGU/L+YGg==" saltValue="aYsNbNwirVdfbZpnR9zITQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FpFaiAt/hj0mRaeMQbB7SwPHtnqdpuLITDAqPUXBp8SuV4Wlwra5XV/V/t2i0Sbqawe5xjZ5939KAYfLbYVJpg==" saltValue="UA3tAN5V2NAz5u+7HUg5VA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
update: add 2 new stationnements
</commit_message>
<xml_diff>
--- a/static/files/stationnements.xlsx
+++ b/static/files/stationnements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AE805E-6EAD-49C3-8DDB-D96EF11D8479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E714209-62DD-4AE2-9C7D-DB41D490FA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>2 roues en extérieur</t>
+  </si>
+  <si>
+    <t>Parking double en sous-sol</t>
+  </si>
+  <si>
+    <t>Parking double en superstructure</t>
   </si>
 </sst>
 </file>
@@ -422,8 +428,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A13" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:A13" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A15" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A15" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Type de stationnement" dataDxfId="0"/>
   </tableColumns>
@@ -731,7 +737,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1030,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3CE0EFE-E6CE-4378-AA4C-1579236482F7}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$13</xm:f>
+            <xm:f>Data!$A$2:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A51</xm:sqref>
         </x14:dataValidation>
@@ -1096,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1178,11 +1184,23 @@
         <v>22</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9cMnaLp5676zm7DSAd618txPB3vEOiBvmm7Gfw8IlWuPS+af/jmvKhvbjtcQ6k5nxAKXooyiVipG4iDLmV+AtQ==" saltValue="6bEwwm21P3CB6ppYmDA+sA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kN9zbrO8UkQG3qPhMbkPJu9FQwSnuOFbEFk4QgplDXlafUbM9XFl+FsbZHLl9faEsm0wyXZeTmQyQXStsAn/qA==" saltValue="9txwQXzZxjSJ1yvQ8cqUZw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
S510 adjustement before mep (#257)
* update: migrate status "transmise" to "signée" + Fiche CAF

* fix: redirection for signed conventions

* update: resiliation date on recap

* update: back to instruction for signed conventions and permission to upload or resiliate conventions only for instructeurs

* update: add 2 new stationnements

* Fix test

* update : fix tewt services + date validation/resiliation visible by everybody

* fix test back to instruction

* fix test redirect signed
</commit_message>
<xml_diff>
--- a/static/files/stationnements.xlsx
+++ b/static/files/stationnements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AE805E-6EAD-49C3-8DDB-D96EF11D8479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E714209-62DD-4AE2-9C7D-DB41D490FA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>2 roues en extérieur</t>
+  </si>
+  <si>
+    <t>Parking double en sous-sol</t>
+  </si>
+  <si>
+    <t>Parking double en superstructure</t>
   </si>
 </sst>
 </file>
@@ -422,8 +428,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A13" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:A13" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A15" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A15" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Type de stationnement" dataDxfId="0"/>
   </tableColumns>
@@ -731,7 +737,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1030,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3CE0EFE-E6CE-4378-AA4C-1579236482F7}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$13</xm:f>
+            <xm:f>Data!$A$2:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A51</xm:sqref>
         </x14:dataValidation>
@@ -1096,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1178,11 +1184,23 @@
         <v>22</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9cMnaLp5676zm7DSAd618txPB3vEOiBvmm7Gfw8IlWuPS+af/jmvKhvbjtcQ6k5nxAKXooyiVipG4iDLmV+AtQ==" saltValue="6bEwwm21P3CB6ppYmDA+sA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kN9zbrO8UkQG3qPhMbkPJu9FQwSnuOFbEFk4QgplDXlafUbM9XFl+FsbZHLl9faEsm0wyXZeTmQyQXStsAn/qA==" saltValue="9txwQXzZxjSJ1yvQ8cqUZw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add type of stationnement : by blocs or accolated
</commit_message>
<xml_diff>
--- a/static/files/stationnements.xlsx
+++ b/static/files/stationnements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E714209-62DD-4AE2-9C7D-DB41D490FA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAB720B-316C-2D4A-93DC-675B4AD122FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Stationnements" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Parking double en superstructure</t>
+  </si>
+  <si>
+    <t>Garages individuels jumelés par blocs de 2</t>
+  </si>
+  <si>
+    <t>Place de parking accolée à chaque garage</t>
   </si>
 </sst>
 </file>
@@ -214,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -249,17 +255,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -310,35 +305,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -428,8 +421,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A15" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:A15" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A17" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A17" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Type de stationnement" dataDxfId="0"/>
   </tableColumns>
@@ -438,9 +431,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -478,7 +471,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -584,7 +577,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -726,7 +719,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -736,287 +729,285 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="30.875" customWidth="1"/>
+    <col min="1" max="3" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
-      <c r="B3" s="12"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
+    <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="10"/>
       <c r="D6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
-      <c r="B7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="9"/>
       <c r="D7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
-      <c r="B9" s="12"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
-      <c r="B13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
-      <c r="B15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
-      <c r="B17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
-      <c r="B19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="12"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="10"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
-      <c r="B23" s="12"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
-      <c r="B27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="10"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
-      <c r="B29" s="12"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="9"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="10"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
-      <c r="B31" s="12"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="9"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="10"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
-      <c r="B33" s="12"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="9"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="10"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
-      <c r="B35" s="12"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="9"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="10"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
-      <c r="B37" s="12"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="9"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="10"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
-      <c r="B39" s="12"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="9"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="10"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
-      <c r="B41" s="12"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="9"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
-      <c r="B43" s="12"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="9"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="10"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
-      <c r="B45" s="12"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="9"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="10"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="B47" s="12"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="9"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
       <c r="C48" s="10"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
-      <c r="B49" s="12"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="9"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
       <c r="C50" s="10"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1028,9 +1019,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3CE0EFE-E6CE-4378-AA4C-1579236482F7}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{31351FEE-EEB5-0D41-8B16-4110E99BCFD9}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$15</xm:f>
+            <xm:f>Data!$A$2:$A$17</xm:f>
           </x14:formula1>
           <xm:sqref>A3:A51</xm:sqref>
         </x14:dataValidation>
@@ -1048,48 +1039,48 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -1102,100 +1093,108 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="15">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kN9zbrO8UkQG3qPhMbkPJu9FQwSnuOFbEFk4QgplDXlafUbM9XFl+FsbZHLl9faEsm0wyXZeTmQyQXStsAn/qA==" saltValue="9txwQXzZxjSJ1yvQ8cqUZw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="PYQOo5uLTdwjuCpUSMMm7nnCUot2baLVwKk3ZBn9gohweLzGsu9N9jsEFzS1hVfwXK9LEbXh2Z96Kh1G6sIBTA==" saltValue="sBdKlTpg++QCHTyUie+JlQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>